<commit_message>
Sco/UK test comparison updated and being published.
</commit_message>
<xml_diff>
--- a/data/R-Table5-Testing.xlsx
+++ b/data/R-Table5-Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\githome\TTS-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF685624-1155-4C2D-BB54-95C9B693B536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C73B1E-C37D-4205-9918-72E7F736BF03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{93D57720-AC84-4EF6-A2D3-6D35E30BD1F9}"/>
+    <workbookView xWindow="8550" yWindow="240" windowWidth="17145" windowHeight="16080" xr2:uid="{93D57720-AC84-4EF6-A2D3-6D35E30BD1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="R-Table5-Testing" sheetId="1" r:id="rId1"/>
@@ -857,8 +857,8 @@
   </sheetPr>
   <dimension ref="A1:AJ285"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A230" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B280" sqref="B280:D280"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A242" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C279" sqref="C279:D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23588,12 +23588,8 @@
       <c r="B279" s="70">
         <v>393216</v>
       </c>
-      <c r="C279" s="92">
-        <v>595.78181818181815</v>
-      </c>
-      <c r="D279" s="91">
-        <v>465.55779220779215</v>
-      </c>
+      <c r="C279" s="92"/>
+      <c r="D279" s="91"/>
       <c r="E279" s="49">
         <v>1110733</v>
       </c>
@@ -23678,12 +23674,8 @@
       <c r="B280" s="70">
         <v>393216</v>
       </c>
-      <c r="C280" s="92">
-        <v>595.78181818181815</v>
-      </c>
-      <c r="D280" s="91">
-        <v>465.55779220779215</v>
-      </c>
+      <c r="C280" s="92"/>
+      <c r="D280" s="91"/>
       <c r="E280" s="49">
         <v>1116611</v>
       </c>

</xml_diff>